<commit_message>
Changed annualized historic data to % chg year ago. Scaled GDPactual, trend, & growth.
</commit_message>
<xml_diff>
--- a/Input_Data/Median_RGDP_Level.xlsx
+++ b/Input_Data/Median_RGDP_Level.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2b09e99cea646701/Bloomberg/Projects/FOMC/FOMC Paper/FOMC_Sentiment_Macro_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2b09e99cea646701/Bloomberg/Projects/FOMC/FOMC Paper/FOMC_Sentiment_Macro_Data/Input_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="8_{C32186B1-655E-4909-AE3B-DE016166CB0D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AFCC83F9-D505-4A04-B4E5-BD9DB47D5D21}"/>
+  <xr:revisionPtr revIDLastSave="143" documentId="8_{C32186B1-655E-4909-AE3B-DE016166CB0D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F094377D-0A51-498B-BA22-00069142F993}"/>
   <bookViews>
-    <workbookView xWindow="20064" yWindow="36" windowWidth="10704" windowHeight="16656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Median_Level" sheetId="1" r:id="rId1"/>
@@ -76,9 +76,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="##0"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="167" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -119,7 +120,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -136,6 +137,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -272,11 +276,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L211"/>
+  <dimension ref="A1:L227"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A152" sqref="A152:XFD152"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.05" customHeight="1"/>
@@ -8270,6 +8274,62 @@
       <c r="E211" s="5"/>
       <c r="F211" s="5"/>
     </row>
+    <row r="220" spans="1:12" ht="13.05" customHeight="1">
+      <c r="A220" s="3"/>
+      <c r="B220" s="3"/>
+      <c r="C220" s="5"/>
+      <c r="D220" s="6"/>
+      <c r="E220" s="6"/>
+    </row>
+    <row r="221" spans="1:12" ht="13.05" customHeight="1">
+      <c r="A221" s="3"/>
+      <c r="B221" s="3"/>
+      <c r="C221" s="5"/>
+      <c r="D221" s="6"/>
+      <c r="E221" s="6"/>
+    </row>
+    <row r="222" spans="1:12" ht="13.05" customHeight="1">
+      <c r="A222" s="3"/>
+      <c r="B222" s="3"/>
+      <c r="C222" s="5"/>
+      <c r="D222" s="6"/>
+      <c r="E222" s="6"/>
+    </row>
+    <row r="223" spans="1:12" ht="13.05" customHeight="1">
+      <c r="A223" s="3"/>
+      <c r="B223" s="3"/>
+      <c r="C223" s="5"/>
+      <c r="D223" s="6"/>
+      <c r="E223" s="6"/>
+    </row>
+    <row r="224" spans="1:12" ht="13.05" customHeight="1">
+      <c r="A224" s="3"/>
+      <c r="B224" s="3"/>
+      <c r="C224" s="5"/>
+      <c r="D224" s="6"/>
+      <c r="E224" s="6"/>
+    </row>
+    <row r="225" spans="1:5" ht="13.05" customHeight="1">
+      <c r="A225" s="3"/>
+      <c r="B225" s="3"/>
+      <c r="C225" s="5"/>
+      <c r="D225" s="6"/>
+      <c r="E225" s="6"/>
+    </row>
+    <row r="226" spans="1:5" ht="13.05" customHeight="1">
+      <c r="A226" s="3"/>
+      <c r="B226" s="3"/>
+      <c r="C226" s="5"/>
+      <c r="D226" s="6"/>
+      <c r="E226" s="6"/>
+    </row>
+    <row r="227" spans="1:5" ht="13.05" customHeight="1">
+      <c r="A227" s="3"/>
+      <c r="B227" s="3"/>
+      <c r="C227" s="5"/>
+      <c r="D227" s="6"/>
+      <c r="E227" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>